<commit_message>
Test cases for Login functionality
</commit_message>
<xml_diff>
--- a/Open Cart Project/Softer_Testing_Project1.xlsx
+++ b/Open Cart Project/Softer_Testing_Project1.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niraj dhakal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\niraj dhakal\Desktop\Manual Testing\Open Cart Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Senario" sheetId="1" r:id="rId1"/>
     <sheet name="Home" sheetId="4" r:id="rId2"/>
+    <sheet name="Login" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="182">
   <si>
     <t>Project Name</t>
   </si>
@@ -430,12 +431,376 @@
   <si>
     <t>Test Cases For Home</t>
   </si>
+  <si>
+    <t>Test Cases for Login</t>
+  </si>
+  <si>
+    <t>TC_Log_01</t>
+  </si>
+  <si>
+    <t>Check all the fields and Login button are clickable in the login page</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt;Click Login -&gt;Visit Login page-&gt; Click E-mail Address -&gt; Click Password -&gt; Click Login</t>
+  </si>
+  <si>
+    <t>Should be able to click all the fields and login button</t>
+  </si>
+  <si>
+    <t>TC_Log_02</t>
+  </si>
+  <si>
+    <t>Verify Email Address values can be copied</t>
+  </si>
+  <si>
+    <t>as@yahoo.com</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt;Click Login -&gt;Visit Login page-&gt; Enter E-mail Address -&gt; Copy E-mail Adress -&gt;Paste the value in other place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be able to copy email as copied values can be pasted </t>
+  </si>
+  <si>
+    <t>TC_Log_03</t>
+  </si>
+  <si>
+    <t>Verify Password values can not be copied</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt;Click Login -&gt;Visit Login page-&gt; Enter Password -&gt; Copy Password -&gt;Paste the copied value in other place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be able to copy pasword as copied values can not be pasted </t>
+  </si>
+  <si>
+    <t>TC_Log_04</t>
+  </si>
+  <si>
+    <t>Verify Password field does not show value when input has taken</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt;Click Login -&gt;Visit Login page-&gt; Enter Password -&gt; Check password visibility</t>
+  </si>
+  <si>
+    <t>Should be able to hide password when password input has taken</t>
+  </si>
+  <si>
+    <t>TC_Log_05</t>
+  </si>
+  <si>
+    <t>Check UI of Login page</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt;Click Login -&gt;Visit Login page-&gt; Check UI of login page</t>
+  </si>
+  <si>
+    <t>Should be able to view proper UI</t>
+  </si>
+  <si>
+    <t>TC_Log_06</t>
+  </si>
+  <si>
+    <t>Verify Login with registered E-Mail Address and valid Password</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Email:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  Riya.ritu@yahoo.com,                                                   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Password: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">riyaritu345%           </t>
+    </r>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Login -&gt; Visit Login page -&gt; Enter E-Mail Address - &gt; Enter Password -&gt;  Click Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be able to login and My Account page will be loaded </t>
+  </si>
+  <si>
+    <t>TC_Log_07</t>
+  </si>
+  <si>
+    <t>Verify Login with registered E-Mail Address and invalid password</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Email:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ami@gmail.com,   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Password:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> rtyfj68</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Should not be able to login and a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>pop-up message will be shown "Warning: No match for E-Mail Address and/or Password."</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_Log_08</t>
+  </si>
+  <si>
+    <t>Verify Login with unregistered E-mail Address and valid password</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Email:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> gjugffkf@gmail.com, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Password: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ami4</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_Log_09</t>
+  </si>
+  <si>
+    <t>Verify Login with unregistered E-mail Address and invalid password</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Email:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> hfk@yahoo.com,                                            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Password: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>NJHYUIKJhYTGFR$%^&amp;*98</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_Log_10</t>
+  </si>
+  <si>
+    <t>Verify Login with empty fields</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Login -&gt; Visit Login page -&gt; Keep E-mail Address and Password field blank -&gt;  Click Login</t>
+  </si>
+  <si>
+    <t>TC_Log_11</t>
+  </si>
+  <si>
+    <t>Verify Login with one user's registered email and another user's password</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Email:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Riya.ritu@yahoo.com                                        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  Password: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ami4       </t>
+    </r>
+  </si>
+  <si>
+    <t>TC_Log_12</t>
+  </si>
+  <si>
+    <t>Verify Forgot Password hyperlink is taking to Forgot Password page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View opencart home page-&gt; Click My Account from header-&gt; Click Login -&gt; Visit Login page -&gt; Click Forgot Password </t>
+  </si>
+  <si>
+    <t>Should be able to display Forgot Password page</t>
+  </si>
+  <si>
+    <t>TC_Log_13</t>
+  </si>
+  <si>
+    <t>Verify New Customer Continue hyperlink is taking to the Register page</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Login -&gt; Visit Login page -&gt; Click Continue in New Customer box</t>
+  </si>
+  <si>
+    <t>Should be able to display Register Account page</t>
+  </si>
+  <si>
+    <t>TC_Log_14</t>
+  </si>
+  <si>
+    <t>Check all the clickable links in the breadcrumbs of Login page can be visited</t>
+  </si>
+  <si>
+    <t>Should be able to visit all the pages in the breadcrumbs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,8 +879,32 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4472C4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -594,8 +983,20 @@
         <bgColor rgb="FF9FD5F1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E2F3"/>
+        <bgColor rgb="FFD9E2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF87B38E"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -744,12 +1145,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -843,6 +1255,23 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1126,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,7 +1729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>27</v>
       </c>
@@ -1314,7 +1743,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>29</v>
       </c>
@@ -1328,7 +1757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>31</v>
       </c>
@@ -1342,7 +1771,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>33</v>
       </c>
@@ -1356,7 +1785,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>35</v>
       </c>
@@ -1370,7 +1799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>37</v>
       </c>
@@ -1384,7 +1813,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>39</v>
       </c>
@@ -1398,7 +1827,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>41</v>
       </c>
@@ -1412,7 +1841,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>43</v>
       </c>
@@ -1426,7 +1855,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>45</v>
       </c>
@@ -1440,7 +1869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>47</v>
       </c>
@@ -1454,7 +1883,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>50</v>
       </c>
@@ -1468,7 +1897,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>52</v>
       </c>
@@ -1482,7 +1911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>54</v>
       </c>
@@ -1496,7 +1925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>56</v>
       </c>
@@ -1510,7 +1939,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>58</v>
       </c>
@@ -1524,7 +1953,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>60</v>
       </c>
@@ -1538,7 +1967,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>62</v>
       </c>
@@ -1552,7 +1981,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>64</v>
       </c>
@@ -1566,7 +1995,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>66</v>
       </c>
@@ -1580,7 +2009,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>68</v>
       </c>
@@ -1594,7 +2023,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>70</v>
       </c>
@@ -1608,7 +2037,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>72</v>
       </c>
@@ -1622,7 +2051,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>74</v>
       </c>
@@ -1660,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1918,4 +2347,357 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D7:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="40" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="52.5546875" customWidth="1"/>
+    <col min="9" max="9" width="46.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="39"/>
+    </row>
+    <row r="8" spans="4:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D8" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+      <c r="D9" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="D10" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="D11" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="35">
+        <v>456789</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="D12" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="35">
+        <v>347867</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="D13" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="I13" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+      <c r="D14" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+      <c r="D15" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+      <c r="D16" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+      <c r="D17" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="D18" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+      <c r="D19" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="D20" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="D21" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+      <c r="D22" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D7:I7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F9" r:id="rId1"/>
+    <hyperlink ref="F10" r:id="rId2"/>
+    <hyperlink ref="F11" r:id="rId3"/>
+    <hyperlink ref="F12" r:id="rId4"/>
+    <hyperlink ref="F13" r:id="rId5"/>
+    <hyperlink ref="F14" r:id="rId6"/>
+    <hyperlink ref="F15" r:id="rId7"/>
+    <hyperlink ref="F16" r:id="rId8"/>
+    <hyperlink ref="F17" r:id="rId9"/>
+    <hyperlink ref="F18" r:id="rId10"/>
+    <hyperlink ref="F19" r:id="rId11"/>
+    <hyperlink ref="F20" r:id="rId12"/>
+    <hyperlink ref="F21" r:id="rId13"/>
+    <hyperlink ref="F22" r:id="rId14"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test cases for Register functionality
</commit_message>
<xml_diff>
--- a/Open Cart Project/Softer_Testing_Project1.xlsx
+++ b/Open Cart Project/Softer_Testing_Project1.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Senario" sheetId="1" r:id="rId1"/>
     <sheet name="Home" sheetId="4" r:id="rId2"/>
     <sheet name="Login" sheetId="5" r:id="rId3"/>
+    <sheet name="Register" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="281">
   <si>
     <t>Project Name</t>
   </si>
@@ -766,15 +767,6 @@
     <t>TC_Log_12</t>
   </si>
   <si>
-    <t>Verify Forgot Password hyperlink is taking to Forgot Password page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">View opencart home page-&gt; Click My Account from header-&gt; Click Login -&gt; Visit Login page -&gt; Click Forgot Password </t>
-  </si>
-  <si>
-    <t>Should be able to display Forgot Password page</t>
-  </si>
-  <si>
     <t>TC_Log_13</t>
   </si>
   <si>
@@ -794,13 +786,570 @@
   </si>
   <si>
     <t>Should be able to visit all the pages in the breadcrumbs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Email:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Riya.ritu@yahoo.com                                        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  Password: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ami5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>TC_Reg_01</t>
+  </si>
+  <si>
+    <t>Check the UI of Register Account</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt;  Check UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be able to view proper UI of register page   </t>
+  </si>
+  <si>
+    <t>TC_Reg_02</t>
+  </si>
+  <si>
+    <t>Verify account registration when First Name field input has letters and fullstop as special characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Md.Akkas                  </t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt; Enter First Name - &gt;Fill rest of the fields with valid information -&gt; Choose any options from  Newsletter -&gt; Check mark  privacy policy -&gt; Click Continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Should be able to register and logged in and Your Account Has Been Created page will  redirect and My Account page will redirect.</t>
+  </si>
+  <si>
+    <t>TC_Reg_03</t>
+  </si>
+  <si>
+    <t>Verify account registration when First Name field input range is between 1 to 32 characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1 character : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">a                                                                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 32 character :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Abchgfrtyuikljnmhgytrewqasdfghjk</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_Reg_04</t>
+  </si>
+  <si>
+    <t>Verify account registration when Last Name field input has spaces between characters</t>
+  </si>
+  <si>
+    <t>R a n a k</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt; Enter First Name - &gt; Fill rest of the fields with valid information -&gt;  Choose any options from  Newsletter -&gt; Check mark  privacy policy -&gt; Click Continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Should not be able to register and logged in and   error messege will be shown under First Nam field "First Name does not appear to be valid!"  </t>
+  </si>
+  <si>
+    <t>TC_Reg_05</t>
+  </si>
+  <si>
+    <t>Verify account registration when First Name field input start with small letters</t>
+  </si>
+  <si>
+    <t>ena</t>
+  </si>
+  <si>
+    <t>TC_Reg_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify account registration when Last Name field input has integers and special characters except fullstop,hyphen,apostrophe s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">@!#435658#$%^34        </t>
+  </si>
+  <si>
+    <t>TC_Reg_07</t>
+  </si>
+  <si>
+    <t>Verify account registration when First Name field input has 33 characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">33 character : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Abchgfrtyuikljnmhgytrewqasdfghjkj</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Should not be able to register and logged in and   error messege will be shown under First Nam field "First Name must be between 1 and 32 characters!"</t>
+  </si>
+  <si>
+    <t>TC_Reg_08</t>
+  </si>
+  <si>
+    <t>Verify account registration when Last Name field input has letters, spaces and fullstop,hyphen and apostrophe s as special characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O'Brian,Van Buren,Smith-Brown     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt; Enter Last Name - &gt; Fill rest of the fields with valid information  -&gt; Choose any options from  Newsletter -&gt;Check mark  privacy policy -&gt; Click Continue </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Should be able to register and logged in and Your Account Has Been Created page will redirect and My Account page will redirect.</t>
+  </si>
+  <si>
+    <t>TC_Reg_09</t>
+  </si>
+  <si>
+    <t>Verify account registration when Last Name field input range is between 1 to 32 characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1 character :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> b                                                                                                            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    32 character :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Abchgfrtyuikljnmhgytrewqasdfghjk</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_Reg_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  R  y  a  n  k  </t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt; Enter Last Name- &gt; Fill rest of the fields with valid information -&gt;  Choose any options from  Newsletter -&gt; Check mark  privacy policy -&gt; Click Continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Should not be able to register and logged in and  error messege will be shown under Last Name field "Last Name does not appear to be valid!"</t>
+  </si>
+  <si>
+    <t>TC_Reg_11</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>45!@#$^*567%$56</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_Reg_12</t>
+  </si>
+  <si>
+    <t>Verify account registration when Last Name field input start with small letters</t>
+  </si>
+  <si>
+    <t>rani</t>
+  </si>
+  <si>
+    <t>TC_Reg_13</t>
+  </si>
+  <si>
+    <t>Verify account registration when Last Name field input has 33 characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0563C1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>33 character :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Abchgfrtyuikljnmhgytrewqasdfghjkj</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_Reg_14</t>
+  </si>
+  <si>
+    <t>Verify account registration when  E-Mail field input has letters,integers and fullstop,hyphen,underscore as special characers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no-riya.dh_ah99@gmail64.gov.bd                                                                                                                                </t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt; Enter E-Mail - &gt; Fill rest of the fields with valid information -&gt;  Choose any options from  Newsletter -&gt; Check mark  privacy policy -&gt; Click Continue</t>
+  </si>
+  <si>
+    <t>TC_Reg_15</t>
+  </si>
+  <si>
+    <t>Verify account registration when  E-Mail field input has only Block letters</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ERGF@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>TC_Reg_16</t>
+  </si>
+  <si>
+    <t>Verify account registration when E-mail field use registered email</t>
+  </si>
+  <si>
+    <t>k@yahoo.com</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt; Enter E-mail - &gt; Fill rest of the fields with valid information -&gt;  Choose any options from  Newsletter -&gt; Check mark  privacy policy -&gt; Click Continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Should not be able to register and logged in  and pop up messege will be shown  " Warning: E-Mail Address is already registered!"</t>
+  </si>
+  <si>
+    <t>TC_Reg_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify account registration when  E-Mail field has only special characters except fullstop,hyphen,underscore </t>
+  </si>
+  <si>
+    <t>%@@^%^^*&amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Should not be able to register and logged in  and error messege will be shown under E-mail field "E-Mail Address does not appear to be valid!" </t>
+  </si>
+  <si>
+    <t>TC_Reg_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify account registration when  E-Mail field input has spaces </t>
+  </si>
+  <si>
+    <t>ahana na na@outlook.com</t>
+  </si>
+  <si>
+    <t>TC_Reg_19</t>
+  </si>
+  <si>
+    <t>Verify account registration when Password field input has letters,special characters,integers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABtyg65%$#@y68#!                                                       </t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt; Enter Password - &gt; Fill rest of the fields with valid information -&gt;  Choose any options from  Newsletter -&gt; Check mark  privacy policy -&gt; Click Continue</t>
+  </si>
+  <si>
+    <t>TC_Reg_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify account registration when Password field input has spaces </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5678  965 %$#                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Should not be able to register and logged in and error message will be shown under Password field "Password has invalid input"</t>
+  </si>
+  <si>
+    <t>TC_Reg_21</t>
+  </si>
+  <si>
+    <t>Verify account registration when Password field input range is between 4 to 20 characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4 characters </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: asdg                                                             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  20 characters </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>: asdghjuytre45678#$%^</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_Reg_22</t>
+  </si>
+  <si>
+    <t>Verify account registration when Password field input has 3 characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    3 characters :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> abc </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Should not be able to register and logged in  and pop up messege will be shown  "Password must be between 4 and 20 characters!"</t>
+  </si>
+  <si>
+    <t>TC_Reg_23</t>
+  </si>
+  <si>
+    <t>Verify account registration when Password field input has 21 characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">21 characters : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>asdghjuytre45678#$%^u</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_Reg_24</t>
+  </si>
+  <si>
+    <t>Check confirmation mail is sent to the given email after registering an account</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt;  Fill up every field with valid information&gt;  Choose any options from  Newsletter -&gt; Check mark  privacy policy -&gt;  Click Continue -&gt; Check mail for confirmation mail.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be able to register and logged in and will redirect to account successs page   and will give a confirmation mail in the given mail address                                                                </t>
+  </si>
+  <si>
+    <t>TC_Reg_25</t>
+  </si>
+  <si>
+    <t>Verify all the hyperlinks in the Register Account and Account success page</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt; Check all the hyperlinks -&gt; Filling necessary fields visit Account success page -&gt; Check all the hyperlinks</t>
+  </si>
+  <si>
+    <t>All the hyperlinks should be able to work</t>
+  </si>
+  <si>
+    <t>TC_Reg_26</t>
+  </si>
+  <si>
+    <t>Verify account registration when  privacy policy box is not ticked</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt;  Fill all the fields with valid information -&gt;  Choose any options from  Newsletter -&gt; Click Continue</t>
+  </si>
+  <si>
+    <t>Should not be able to register  and a pop up message will be shown  "Warning: You must agree to the Privacy Policy!"</t>
+  </si>
+  <si>
+    <t>TC_Reg_27</t>
+  </si>
+  <si>
+    <t>Verify account registration if all the mandatory field remain empty</t>
+  </si>
+  <si>
+    <t>View opencart home page-&gt; Click My Account from header-&gt; Click Register -&gt; Visit register account page -&gt;  Keep all the fields empty -&gt;  Choose any options from  Newsletter -&gt; Check mark  privacy policy -&gt;  Click Continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should not be able to register  and warning messages will be shown  under every mandatory field.  For First Name, "First Name must be between 1 and 32 characters!"                                                                                                                          Last Name,"Last Name must be between 1 and 32 characters!"                                                                                                                                                                   E-Mail,"E-Mail Address does not appear to be valid!"                                                                                            Password,"Password must be between 4 and 20 characters!"                                                                                         </t>
+  </si>
+  <si>
+    <t>Test Cases for Register Functionality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -903,8 +1452,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -992,6 +1560,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF87B38E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFD965"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFF7CAAC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFF8BE9E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF87B38E"/>
       </patternFill>
     </fill>
@@ -1159,119 +1757,169 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1553,10 +2201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I41"/>
+  <dimension ref="A2:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1625,12 +2273,9 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="18" t="s">
-        <v>12</v>
-      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -1638,444 +2283,450 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:9" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="C13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E13" s="17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="C14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="14">
+      <c r="D14" s="14">
         <v>10</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="15" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="10">
+      <c r="D15" s="10">
         <v>16</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    </row>
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="10">
+      <c r="D16" s="10">
         <v>10</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+    <row r="17" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="10">
+      <c r="D17" s="10">
         <v>5</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+    <row r="18" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="10">
+      <c r="D18" s="10">
         <v>27</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+    <row r="19" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="8">
+      <c r="D19" s="8">
         <v>14</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+    <row r="20" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="8">
+      <c r="D20" s="8">
         <v>10</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+    <row r="21" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="8">
+      <c r="D21" s="8">
         <v>5</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+    <row r="22" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="8">
+      <c r="D22" s="8">
         <v>10</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="E22" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+    <row r="23" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="C23" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="8">
+      <c r="D23" s="8">
         <v>18</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+    <row r="24" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="C24" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="8">
+      <c r="D24" s="8">
         <v>10</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="E24" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+    <row r="25" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="8">
+      <c r="D25" s="8">
         <v>10</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+    <row r="26" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="8">
+      <c r="D26" s="8">
         <v>11</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+    <row r="27" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="8">
+      <c r="D27" s="8">
         <v>10</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="E27" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+    <row r="28" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="8">
+      <c r="D28" s="8">
         <v>10</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+    <row r="29" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="8">
+      <c r="D29" s="8">
         <v>10</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+    <row r="30" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="8">
+      <c r="D30" s="8">
         <v>10</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+    <row r="31" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B31" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="8">
+      <c r="D31" s="8">
         <v>10</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+    <row r="32" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B32" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="C32" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="8">
+      <c r="D32" s="8">
         <v>10</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+    <row r="33" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B33" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="8">
+      <c r="D33" s="8">
         <v>40</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
+    <row r="34" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B34" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="C34" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C32" s="8">
+      <c r="D34" s="8">
         <v>11</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="E34" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
+    <row r="35" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B35" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="C35" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="8">
+      <c r="D35" s="8">
         <v>23</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+    <row r="36" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="8">
+      <c r="D36" s="8">
         <v>20</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
+    <row r="37" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="C37" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="8">
+      <c r="D37" s="8">
         <v>15</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
+    <row r="38" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="C38" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="8">
+      <c r="D38" s="8">
         <v>15</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
+    <row r="39" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B39" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C37" s="8">
+      <c r="D39" s="8">
         <v>13</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+    <row r="40" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B40" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="C40" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="8">
+      <c r="D40" s="8">
         <v>17</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
+    <row r="41" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="8">
+      <c r="D41" s="8">
         <v>10</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
+    <row r="42" spans="2:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="C42" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="8">
+      <c r="D42" s="8">
         <v>10</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
+    <row r="43" spans="2:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="C43" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="8">
+      <c r="D43" s="8">
         <v>23</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="E43" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2353,7 +3004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D7:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7:I7"/>
     </sheetView>
   </sheetViews>
@@ -2557,7 +3208,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:9" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="34" t="s">
         <v>162</v>
       </c>
@@ -2577,7 +3228,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="4:9" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="34" t="s">
         <v>165</v>
       </c>
@@ -2597,7 +3248,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D19" s="34" t="s">
         <v>168</v>
       </c>
@@ -2617,32 +3268,32 @@
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="4:9" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:9" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="34" t="s">
         <v>171</v>
       </c>
       <c r="E20" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="F20" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="H20" s="23" t="s">
+      <c r="E21" s="28" t="s">
         <v>173</v>
-      </c>
-      <c r="I20" s="26" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="4:9" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="D21" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>176</v>
       </c>
       <c r="F21" s="29" t="s">
         <v>86</v>
@@ -2651,18 +3302,18 @@
         <v>87</v>
       </c>
       <c r="H21" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="28" t="s">
         <v>177</v>
-      </c>
-      <c r="I21" s="26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="22" spans="4:9" ht="288" x14ac:dyDescent="0.3">
-      <c r="D22" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>180</v>
       </c>
       <c r="F22" s="29" t="s">
         <v>86</v>
@@ -2674,7 +3325,7 @@
         <v>153</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2693,11 +3344,637 @@
     <hyperlink ref="F17" r:id="rId9"/>
     <hyperlink ref="F18" r:id="rId10"/>
     <hyperlink ref="F19" r:id="rId11"/>
-    <hyperlink ref="F20" r:id="rId12"/>
-    <hyperlink ref="F21" r:id="rId13"/>
-    <hyperlink ref="F22" r:id="rId14"/>
+    <hyperlink ref="F21" r:id="rId12"/>
+    <hyperlink ref="F22" r:id="rId13"/>
+    <hyperlink ref="F20" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C7:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="6" width="41.33203125" customWidth="1"/>
+    <col min="7" max="7" width="48.5546875" customWidth="1"/>
+    <col min="8" max="8" width="42.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:8" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="55" t="s">
+        <v>280</v>
+      </c>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="57"/>
+    </row>
+    <row r="9" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C9" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C10" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C11" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C12" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C13" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C14" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C15" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>202</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C16" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="46" t="s">
+        <v>205</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C17" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>208</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C18" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C19" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="H19" s="41" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C20" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>201</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C21" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="H21" s="41" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C22" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="49" t="s">
+        <v>226</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C23" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="H23" s="41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C24" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="H24" s="41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C25" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>235</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="52" t="s">
+        <v>236</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="H25" s="41" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C26" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="53" t="s">
+        <v>241</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="H26" s="41" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C27" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>244</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="54" t="s">
+        <v>245</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="H27" s="41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C28" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>247</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="51" t="s">
+        <v>248</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="H28" s="41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C29" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>251</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="H29" s="41" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C30" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="D30" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="51" t="s">
+        <v>256</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="H30" s="41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C31" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="51" t="s">
+        <v>259</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="H31" s="41" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C32" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="53" t="s">
+        <v>263</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="H32" s="41" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C33" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="H33" s="41" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C34" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="D34" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="H34" s="43" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C35" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="D35" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="H35" s="41" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="C36" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="D36" s="44" t="s">
+        <v>277</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="H36" s="41" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C7:H7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E11" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="E13" r:id="rId4"/>
+    <hyperlink ref="E14" r:id="rId5"/>
+    <hyperlink ref="E15" r:id="rId6"/>
+    <hyperlink ref="E16" r:id="rId7"/>
+    <hyperlink ref="E17" r:id="rId8"/>
+    <hyperlink ref="E18" r:id="rId9"/>
+    <hyperlink ref="E19" r:id="rId10"/>
+    <hyperlink ref="E20" r:id="rId11"/>
+    <hyperlink ref="E21" r:id="rId12"/>
+    <hyperlink ref="E22" r:id="rId13"/>
+    <hyperlink ref="E23" r:id="rId14"/>
+    <hyperlink ref="F23" r:id="rId15"/>
+    <hyperlink ref="E24" r:id="rId16"/>
+    <hyperlink ref="E25" r:id="rId17"/>
+    <hyperlink ref="E26" r:id="rId18"/>
+    <hyperlink ref="E27" r:id="rId19"/>
+    <hyperlink ref="E28" r:id="rId20"/>
+    <hyperlink ref="E29" r:id="rId21"/>
+    <hyperlink ref="E30" r:id="rId22"/>
+    <hyperlink ref="E31" r:id="rId23"/>
+    <hyperlink ref="E32" r:id="rId24"/>
+    <hyperlink ref="E33" r:id="rId25"/>
+    <hyperlink ref="E34" r:id="rId26"/>
+    <hyperlink ref="E35" r:id="rId27"/>
+    <hyperlink ref="E36" r:id="rId28"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
logout test cases written
</commit_message>
<xml_diff>
--- a/Open Cart Project/Softer_Testing_Project1.xlsx
+++ b/Open Cart Project/Softer_Testing_Project1.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test Senario" sheetId="1" r:id="rId1"/>
     <sheet name="Home" sheetId="4" r:id="rId2"/>
     <sheet name="Login" sheetId="5" r:id="rId3"/>
     <sheet name="Register" sheetId="6" r:id="rId4"/>
+    <sheet name="Logout" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="303">
   <si>
     <t>Project Name</t>
   </si>
@@ -1336,6 +1337,97 @@
   </si>
   <si>
     <t>Test Cases for Register Functionality</t>
+  </si>
+  <si>
+    <t>TC_Logout_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user will logout by clicking Logout option from My Account dropmenu </t>
+  </si>
+  <si>
+    <t>No input</t>
+  </si>
+  <si>
+    <t>View Home page-&gt; Complete Login-&gt;View Header-&gt;Click My Account-&gt;View Dropmenu-&gt; Click Logout</t>
+  </si>
+  <si>
+    <t>Should be able to logout and logout page will be displayed and there Clicking Continue will view Home page</t>
+  </si>
+  <si>
+    <t>TC_Logout_02</t>
+  </si>
+  <si>
+    <t>Verify user will logout by clicking Logout option from My Account right column</t>
+  </si>
+  <si>
+    <t>View Home page-&gt; Complete Login-&gt;View My account-&gt; Click Logout from right column</t>
+  </si>
+  <si>
+    <t>TC_Logout_03</t>
+  </si>
+  <si>
+    <t>Verify UI of Account logout Page</t>
+  </si>
+  <si>
+    <t>View Home page-&gt; Complete Login-&gt;View My account-&gt; Click Logout from right column-&gt; Check UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be able to view proper UI of Logout page </t>
+  </si>
+  <si>
+    <t>TC_Logout_04</t>
+  </si>
+  <si>
+    <t>Check Logout option won't show in My Account dropmenu without logging in</t>
+  </si>
+  <si>
+    <t>View Home page-&gt; View Header-&gt;View My account-&gt; Click My account-&gt; View dropmenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should not be able to view Logout option in the My account dropmenu </t>
+  </si>
+  <si>
+    <t>TC_Logout_05</t>
+  </si>
+  <si>
+    <t>Check Logout option won't show in My Account right column without logging in</t>
+  </si>
+  <si>
+    <t>View Home page-&gt; View Header-&gt;View My account-&gt; Click My account-&gt; Click Login-&gt; View My Account-&gt; View right column of My Account</t>
+  </si>
+  <si>
+    <t>Should not be able to view Logout option in the My account page right column</t>
+  </si>
+  <si>
+    <t>Test Cases for Logout Functionality</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Visit </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>demo.opencart.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and user must be logged in</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1343,13 +1435,6 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1471,8 +1556,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1591,6 +1681,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF87B38E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1757,169 +1859,178 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2203,8 +2314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3019,14 +3130,14 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="39"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
     </row>
     <row r="8" spans="4:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D8" s="33" t="s">
@@ -3068,7 +3179,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="4:9" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D10" s="34" t="s">
         <v>133</v>
       </c>
@@ -3088,7 +3199,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="4:9" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D11" s="34" t="s">
         <v>138</v>
       </c>
@@ -3108,7 +3219,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="4:9" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D12" s="34" t="s">
         <v>142</v>
       </c>
@@ -3128,7 +3239,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="4:9" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D13" s="34" t="s">
         <v>146</v>
       </c>
@@ -3148,7 +3259,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D14" s="34" t="s">
         <v>150</v>
       </c>
@@ -3168,7 +3279,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D15" s="34" t="s">
         <v>155</v>
       </c>
@@ -3188,7 +3299,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="4:9" ht="288" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D16" s="34" t="s">
         <v>159</v>
       </c>
@@ -3357,7 +3468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C7:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:H7"/>
     </sheetView>
   </sheetViews>
@@ -3391,7 +3502,7 @@
       <c r="E9" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="37" t="s">
         <v>81</v>
       </c>
       <c r="G9" s="33" t="s">
@@ -3405,19 +3516,19 @@
       <c r="C10" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="41" t="s">
         <v>181</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="F10" s="42" t="s">
         <v>87</v>
       </c>
       <c r="G10" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="H10" s="38" t="s">
         <v>183</v>
       </c>
     </row>
@@ -3425,19 +3536,19 @@
       <c r="C11" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="41" t="s">
         <v>185</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="F11" s="42" t="s">
         <v>186</v>
       </c>
       <c r="G11" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="38" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3445,19 +3556,19 @@
       <c r="C12" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="41" t="s">
         <v>190</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="42" t="s">
         <v>191</v>
       </c>
       <c r="G12" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="H12" s="41" t="s">
+      <c r="H12" s="38" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3465,19 +3576,19 @@
       <c r="C13" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="41" t="s">
         <v>193</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="46" t="s">
+      <c r="F13" s="43" t="s">
         <v>194</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="38" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3485,19 +3596,19 @@
       <c r="C14" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="41" t="s">
         <v>198</v>
       </c>
       <c r="E14" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="46" t="s">
+      <c r="F14" s="43" t="s">
         <v>199</v>
       </c>
       <c r="G14" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="38" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3505,19 +3616,19 @@
       <c r="C15" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="41" t="s">
         <v>201</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="44" t="s">
         <v>202</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="38" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3525,19 +3636,19 @@
       <c r="C16" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="41" t="s">
         <v>204</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="43" t="s">
         <v>205</v>
       </c>
       <c r="G16" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="39" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3545,19 +3656,19 @@
       <c r="C17" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="D17" s="41" t="s">
         <v>208</v>
       </c>
       <c r="E17" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="45" t="s">
+      <c r="F17" s="42" t="s">
         <v>209</v>
       </c>
       <c r="G17" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="H17" s="41" t="s">
+      <c r="H17" s="38" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3565,19 +3676,19 @@
       <c r="C18" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="41" t="s">
         <v>213</v>
       </c>
       <c r="E18" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="45" t="s">
+      <c r="F18" s="42" t="s">
         <v>214</v>
       </c>
       <c r="G18" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="H18" s="41" t="s">
+      <c r="H18" s="38" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3585,19 +3696,19 @@
       <c r="C19" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="41" t="s">
         <v>193</v>
       </c>
       <c r="E19" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="48" t="s">
+      <c r="F19" s="45" t="s">
         <v>216</v>
       </c>
       <c r="G19" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="38" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3605,19 +3716,19 @@
       <c r="C20" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="41" t="s">
         <v>201</v>
       </c>
       <c r="E20" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="48" t="s">
+      <c r="F20" s="45" t="s">
         <v>220</v>
       </c>
       <c r="G20" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="H20" s="41" t="s">
+      <c r="H20" s="38" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3625,19 +3736,19 @@
       <c r="C21" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="D21" s="44" t="s">
+      <c r="D21" s="41" t="s">
         <v>222</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="F21" s="45" t="s">
         <v>223</v>
       </c>
       <c r="G21" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="H21" s="41" t="s">
+      <c r="H21" s="38" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3645,19 +3756,19 @@
       <c r="C22" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="41" t="s">
         <v>225</v>
       </c>
       <c r="E22" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="49" t="s">
+      <c r="F22" s="46" t="s">
         <v>226</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="38" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3665,19 +3776,19 @@
       <c r="C23" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="41" t="s">
         <v>228</v>
       </c>
       <c r="E23" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F23" s="50" t="s">
+      <c r="F23" s="47" t="s">
         <v>229</v>
       </c>
       <c r="G23" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="38" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3685,19 +3796,19 @@
       <c r="C24" s="23" t="s">
         <v>231</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="41" t="s">
         <v>232</v>
       </c>
       <c r="E24" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="51" t="s">
+      <c r="F24" s="48" t="s">
         <v>233</v>
       </c>
       <c r="G24" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="H24" s="41" t="s">
+      <c r="H24" s="38" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3705,19 +3816,19 @@
       <c r="C25" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="D25" s="44" t="s">
+      <c r="D25" s="41" t="s">
         <v>235</v>
       </c>
       <c r="E25" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="52" t="s">
+      <c r="F25" s="49" t="s">
         <v>236</v>
       </c>
       <c r="G25" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="H25" s="41" t="s">
+      <c r="H25" s="38" t="s">
         <v>238</v>
       </c>
     </row>
@@ -3725,19 +3836,19 @@
       <c r="C26" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="D26" s="44" t="s">
+      <c r="D26" s="41" t="s">
         <v>240</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="53" t="s">
+      <c r="F26" s="50" t="s">
         <v>241</v>
       </c>
       <c r="G26" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="H26" s="41" t="s">
+      <c r="H26" s="38" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3745,19 +3856,19 @@
       <c r="C27" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="41" t="s">
         <v>244</v>
       </c>
       <c r="E27" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="54" t="s">
+      <c r="F27" s="51" t="s">
         <v>245</v>
       </c>
       <c r="G27" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="H27" s="41" t="s">
+      <c r="H27" s="38" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3765,19 +3876,19 @@
       <c r="C28" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="41" t="s">
         <v>247</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="51" t="s">
+      <c r="F28" s="48" t="s">
         <v>248</v>
       </c>
       <c r="G28" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="H28" s="41" t="s">
+      <c r="H28" s="38" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3785,19 +3896,19 @@
       <c r="C29" s="23" t="s">
         <v>250</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="41" t="s">
         <v>251</v>
       </c>
       <c r="E29" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="51" t="s">
+      <c r="F29" s="48" t="s">
         <v>252</v>
       </c>
       <c r="G29" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="H29" s="41" t="s">
+      <c r="H29" s="38" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3805,19 +3916,19 @@
       <c r="C30" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="41" t="s">
         <v>255</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="51" t="s">
+      <c r="F30" s="48" t="s">
         <v>256</v>
       </c>
       <c r="G30" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="H30" s="41" t="s">
+      <c r="H30" s="38" t="s">
         <v>211</v>
       </c>
     </row>
@@ -3825,19 +3936,19 @@
       <c r="C31" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="41" t="s">
         <v>258</v>
       </c>
       <c r="E31" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F31" s="51" t="s">
+      <c r="F31" s="48" t="s">
         <v>259</v>
       </c>
       <c r="G31" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="H31" s="41" t="s">
+      <c r="H31" s="38" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3845,19 +3956,19 @@
       <c r="C32" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="D32" s="44" t="s">
+      <c r="D32" s="41" t="s">
         <v>262</v>
       </c>
       <c r="E32" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="53" t="s">
+      <c r="F32" s="50" t="s">
         <v>263</v>
       </c>
       <c r="G32" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="H32" s="41" t="s">
+      <c r="H32" s="38" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3865,19 +3976,19 @@
       <c r="C33" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="D33" s="44" t="s">
+      <c r="D33" s="41" t="s">
         <v>265</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F33" s="52" t="s">
+      <c r="F33" s="49" t="s">
         <v>87</v>
       </c>
       <c r="G33" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="H33" s="41" t="s">
+      <c r="H33" s="38" t="s">
         <v>267</v>
       </c>
     </row>
@@ -3885,19 +3996,19 @@
       <c r="C34" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="D34" s="44" t="s">
+      <c r="D34" s="41" t="s">
         <v>269</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F34" s="52" t="s">
+      <c r="F34" s="49" t="s">
         <v>87</v>
       </c>
       <c r="G34" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="H34" s="43" t="s">
+      <c r="H34" s="40" t="s">
         <v>271</v>
       </c>
     </row>
@@ -3905,19 +4016,19 @@
       <c r="C35" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="D35" s="44" t="s">
+      <c r="D35" s="41" t="s">
         <v>273</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F35" s="52" t="s">
+      <c r="F35" s="49" t="s">
         <v>87</v>
       </c>
       <c r="G35" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="H35" s="41" t="s">
+      <c r="H35" s="38" t="s">
         <v>275</v>
       </c>
     </row>
@@ -3925,19 +4036,19 @@
       <c r="C36" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="D36" s="44" t="s">
+      <c r="D36" s="41" t="s">
         <v>277</v>
       </c>
       <c r="E36" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F36" s="52" t="s">
+      <c r="F36" s="49" t="s">
         <v>87</v>
       </c>
       <c r="G36" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="H36" s="41" t="s">
+      <c r="H36" s="38" t="s">
         <v>279</v>
       </c>
     </row>
@@ -3977,4 +4088,160 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E7:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="67.77734375" customWidth="1"/>
+    <col min="7" max="7" width="70.77734375" customWidth="1"/>
+    <col min="8" max="8" width="44.33203125" customWidth="1"/>
+    <col min="9" max="9" width="46.21875" customWidth="1"/>
+    <col min="10" max="10" width="88" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="5:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="58" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E8" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="5:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E9" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="H9" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="J9" s="60" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="5:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E10" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="J10" s="60" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="5:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E11" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="H11" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="J11" s="60" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="5:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E12" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="J12" s="60" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="5:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E13" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="59" t="s">
+        <v>283</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="J13" s="60" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G9" r:id="rId1"/>
+    <hyperlink ref="G10" r:id="rId2"/>
+    <hyperlink ref="G11" r:id="rId3"/>
+    <hyperlink ref="G12" r:id="rId4"/>
+    <hyperlink ref="G13" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Forgot Password Test cases Written
</commit_message>
<xml_diff>
--- a/Open Cart Project/Softer_Testing_Project1.xlsx
+++ b/Open Cart Project/Softer_Testing_Project1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Test Senario" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Login" sheetId="5" r:id="rId3"/>
     <sheet name="Register" sheetId="6" r:id="rId4"/>
     <sheet name="Logout" sheetId="7" r:id="rId5"/>
+    <sheet name="Forgot_Password" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="338">
   <si>
     <t>Project Name</t>
   </si>
@@ -1428,6 +1429,136 @@
       </rPr>
       <t xml:space="preserve"> and user must be logged in</t>
     </r>
+  </si>
+  <si>
+    <t>TC_ForPass_01</t>
+  </si>
+  <si>
+    <t>Check UI of Forgot Password page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Visit </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>demo.opencart.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and naviagte to the Login page and user should have an valid account</t>
+    </r>
+  </si>
+  <si>
+    <t>View Login Page-&gt; Click Forgot Password-&gt; View UI</t>
+  </si>
+  <si>
+    <t>TC_ForPass_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify reset password with the registered email </t>
+  </si>
+  <si>
+    <t>Riya.ritu@yahoo.com</t>
+  </si>
+  <si>
+    <t>View Login Page-&gt; Click Forgot Password-&gt;Enter E-mail Address-&gt; Click Continue</t>
+  </si>
+  <si>
+    <t>TC_ForPass_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify reset password email is sent to the registered email </t>
+  </si>
+  <si>
+    <t xml:space="preserve">View Login Page-&gt; Click Forgot Password-&gt; Fill up necessary information in the field-&gt; Click Continue-&gt; Check the given email account inbox </t>
+  </si>
+  <si>
+    <t>TC_ForPass_04</t>
+  </si>
+  <si>
+    <t>Verify User can reset password from the password reset email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View Login Page-&gt; Click Forgot Password-&gt; Fill up necessary information in the field-&gt; Click Continue-&gt; Check the given email account inbox -&gt; Click reset password link -&gt; View reset password </t>
+  </si>
+  <si>
+    <t>TC_ForPass_05</t>
+  </si>
+  <si>
+    <t>Verify Forgot Password page breadcrumbs links can be visited</t>
+  </si>
+  <si>
+    <t>View Login Page-&gt; Click Forgot Password -&gt; Click all the links available in the breadcrumbs</t>
+  </si>
+  <si>
+    <t>TC_ForPass_06</t>
+  </si>
+  <si>
+    <t>Verify user can login after resetting their password</t>
+  </si>
+  <si>
+    <t>h@gmail.com</t>
+  </si>
+  <si>
+    <t>View Login Page-&gt; Click Forgot Password-&gt; Fill up necessary information in the field-&gt; Click Continue-&gt; Check the given email account inbox -&gt; Click reset password link -&gt; Reset password-&gt; Go to Login page and enter necessary info with the new reset password-&gt; Click Continue</t>
+  </si>
+  <si>
+    <t>TC_ForPass_07</t>
+  </si>
+  <si>
+    <t>Check all the buttons are working properly</t>
+  </si>
+  <si>
+    <t>View Login Page-&gt; Click Forgot Password -&gt; Click all the buttons available in the page</t>
+  </si>
+  <si>
+    <t>TC_ForPass_08</t>
+  </si>
+  <si>
+    <t>Check error messege is shown when E-mail address is invalid</t>
+  </si>
+  <si>
+    <t>kas@gmail.com</t>
+  </si>
+  <si>
+    <t>View Login Page-&gt; Click Forgot Password-&gt; Enter E-mail Address &gt; Click Continue</t>
+  </si>
+  <si>
+    <t>TC_ForPass_09</t>
+  </si>
+  <si>
+    <t>Verify reset password when E-mail address is empty</t>
+  </si>
+  <si>
+    <t>View Login Page-&gt; Click Forgot Password-&gt;Keep E-mail Address empty-&gt;Click Continue</t>
+  </si>
+  <si>
+    <t>TC_ForPass_10</t>
+  </si>
+  <si>
+    <t>Verify all the hyperlinks in the Forgot Password pages are valid</t>
+  </si>
+  <si>
+    <t>View Login Page-&gt; Click Forgot Password-&gt; Click all the hyperlinks available in the Forgot Password page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Cases For Forgot-Password</t>
   </si>
 </sst>
 </file>
@@ -1861,7 +1992,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2012,6 +2143,15 @@
     <xf numFmtId="0" fontId="10" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2022,14 +2162,11 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2314,7 +2451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3130,14 +3267,14 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="54"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="57"/>
     </row>
     <row r="8" spans="4:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D8" s="33" t="s">
@@ -3483,14 +3620,14 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:8" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="58" t="s">
         <v>280</v>
       </c>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="57"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="60"/>
     </row>
     <row r="9" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C9" s="33" t="s">
@@ -4094,7 +4231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E7:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -4109,7 +4246,7 @@
   </cols>
   <sheetData>
     <row r="7" spans="5:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="52" t="s">
         <v>301</v>
       </c>
     </row>
@@ -4143,13 +4280,13 @@
       <c r="G9" s="29" t="s">
         <v>302</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="53" t="s">
         <v>283</v>
       </c>
       <c r="I9" s="23" t="s">
         <v>284</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="54" t="s">
         <v>285</v>
       </c>
     </row>
@@ -4163,13 +4300,13 @@
       <c r="G10" s="29" t="s">
         <v>302</v>
       </c>
-      <c r="H10" s="59" t="s">
+      <c r="H10" s="53" t="s">
         <v>283</v>
       </c>
       <c r="I10" s="23" t="s">
         <v>288</v>
       </c>
-      <c r="J10" s="60" t="s">
+      <c r="J10" s="54" t="s">
         <v>285</v>
       </c>
     </row>
@@ -4183,13 +4320,13 @@
       <c r="G11" s="29" t="s">
         <v>302</v>
       </c>
-      <c r="H11" s="59" t="s">
+      <c r="H11" s="53" t="s">
         <v>283</v>
       </c>
       <c r="I11" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="J11" s="60" t="s">
+      <c r="J11" s="54" t="s">
         <v>292</v>
       </c>
     </row>
@@ -4203,13 +4340,13 @@
       <c r="G12" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="53" t="s">
         <v>283</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="J12" s="60" t="s">
+      <c r="J12" s="54" t="s">
         <v>296</v>
       </c>
     </row>
@@ -4223,13 +4360,13 @@
       <c r="G13" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="H13" s="59" t="s">
+      <c r="H13" s="53" t="s">
         <v>283</v>
       </c>
       <c r="I13" s="23" t="s">
         <v>299</v>
       </c>
-      <c r="J13" s="60" t="s">
+      <c r="J13" s="54" t="s">
         <v>300</v>
       </c>
     </row>
@@ -4244,4 +4381,265 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C7:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="33.77734375" customWidth="1"/>
+    <col min="5" max="5" width="43.21875" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:8" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="62" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C10" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C11" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>309</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="C12" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>312</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>313</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C13" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C14" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>318</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C15" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>321</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="F15" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C16" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>325</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C17" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>328</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="F17" s="61" t="s">
+        <v>329</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>330</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C18" s="34" t="s">
+        <v>331</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>332</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>333</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C19" s="34" t="s">
+        <v>334</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E11" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="E13" r:id="rId4"/>
+    <hyperlink ref="E14" r:id="rId5"/>
+    <hyperlink ref="E15" r:id="rId6"/>
+    <hyperlink ref="E16" r:id="rId7"/>
+    <hyperlink ref="E17" r:id="rId8"/>
+    <hyperlink ref="E18" r:id="rId9"/>
+    <hyperlink ref="E19" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
order history and payment functionality test cases written
</commit_message>
<xml_diff>
--- a/Open Cart Project/Softer_Testing_Project1.xlsx
+++ b/Open Cart Project/Softer_Testing_Project1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8700" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Test Senario" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Register" sheetId="6" r:id="rId4"/>
     <sheet name="Logout" sheetId="7" r:id="rId5"/>
     <sheet name="Forgot_Password" sheetId="8" r:id="rId6"/>
+    <sheet name="Payment" sheetId="9" r:id="rId7"/>
+    <sheet name="Order" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="417">
   <si>
     <t>Project Name</t>
   </si>
@@ -1559,6 +1561,270 @@
   </si>
   <si>
     <t xml:space="preserve"> Test Cases For Forgot-Password</t>
+  </si>
+  <si>
+    <t>TC_Payment_01</t>
+  </si>
+  <si>
+    <t>Check UI of Payment page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Visit </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>demo.opencart.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and after login My account page is launched</t>
+    </r>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click Payment Methods under My Account section -&gt; View Payment Methods -&gt; Check UI</t>
+  </si>
+  <si>
+    <t>Should be able to view Proper UI</t>
+  </si>
+  <si>
+    <t>TC_Payment_02</t>
+  </si>
+  <si>
+    <t>Check Payment page right side list's links are working properly</t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click Payment Methods under My Account section -&gt; View Payment Methods -&gt; Click right side links</t>
+  </si>
+  <si>
+    <t>Should be able to view respective pages according to the links</t>
+  </si>
+  <si>
+    <t>TC_Payment_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify URL of Payment page </t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click Payment Methods under My Account section -&gt; View Payment Methods -&gt; Check URL</t>
+  </si>
+  <si>
+    <t>Should be able to view Proper URL</t>
+  </si>
+  <si>
+    <t>TC_Payment_04</t>
+  </si>
+  <si>
+    <t>Verify Payment page breadcrumbs home logo is working properly</t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click Payment Methods under My Account section -&gt; View Payment Methods -&gt;  View Breadcrumbs -&gt; Click home logo</t>
+  </si>
+  <si>
+    <t>Should be able to view Home page when home logo will be clicked in the breadcrumbs</t>
+  </si>
+  <si>
+    <t>TC_Payment_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Payment page breadcrumbs 'Account' link can load the account page </t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click Payment Methods under My Account section -&gt; View Payment Methods -&gt;  View Breadcrumbs -&gt; Click Account</t>
+  </si>
+  <si>
+    <t>Should be able to view Account page when Account link will be clicked in the breadcrumbs</t>
+  </si>
+  <si>
+    <t>TC_Payment_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Payment page breadcrumbs 'Payment Methods' link can load the payment page </t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click Payment Methods under My Account section -&gt; View Payment Methods -&gt;  View Breadcrumbs -&gt; Click Payment Methods</t>
+  </si>
+  <si>
+    <t>Should be able to view Payment page when Payment Methods link will be clicked in the breadcrumbs</t>
+  </si>
+  <si>
+    <t>TC_Payment_07</t>
+  </si>
+  <si>
+    <t>Verify If no payment option is not added by user payment page will remain empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View My Account page -&gt; Click Payment Methods under My Account section -&gt; View Payment Methods </t>
+  </si>
+  <si>
+    <t>Should be able to view empty Payment page and in the body of the page a sentence will be shown"You have no payment methods in your account."</t>
+  </si>
+  <si>
+    <t>TC_Payment_08</t>
+  </si>
+  <si>
+    <t>Verify Back button of Payment page can load the Account page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View My Account page -&gt; Click Payment Methods under My Account section -&gt; View Payment Methods-&gt; Click Back </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be able to view Account page when Back button will be clicked </t>
+  </si>
+  <si>
+    <t>TC_Payment_09</t>
+  </si>
+  <si>
+    <t>Check Payment page is secure</t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click Payment Methods under My Account section -&gt; View Payment Methods -&gt; View URL field-&gt; Check lock logo beside URL field</t>
+  </si>
+  <si>
+    <t>Should be able to view the lock logo beside the URL field and clicking the lock logo "Connection is secure" text will be visible</t>
+  </si>
+  <si>
+    <t>TC_Payment_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Payment page favicon is proper </t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click Payment Methods under My Account section -&gt; View Payment Methods -&gt; View favicon in browser tab</t>
+  </si>
+  <si>
+    <t>Should be able to load proper favicon for payment methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Cases For Payment </t>
+  </si>
+  <si>
+    <t>TC_OrderHistory_01</t>
+  </si>
+  <si>
+    <t>Check UI of Order History page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View My Account page -&gt; Click View your order history under My Orders section -&gt; View Order History -&gt;Check UI </t>
+  </si>
+  <si>
+    <t>TC_OrderHistory_02</t>
+  </si>
+  <si>
+    <t>Verify breadcrumb links and right side list links  are working properly</t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click View your order history under My Orders section -&gt; View Order History -&gt; Click breadcrumbs and right side list links</t>
+  </si>
+  <si>
+    <t>Should be able to view all the links respective pages</t>
+  </si>
+  <si>
+    <t>TC_OrderHistory_03</t>
+  </si>
+  <si>
+    <t>Verify Order History view logo will load order information page</t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click View your order history under My Orders  section -&gt; View Order History -&gt; Click View logo</t>
+  </si>
+  <si>
+    <t>Should be able to view  order information page</t>
+  </si>
+  <si>
+    <t>TC_OrderHistory_04</t>
+  </si>
+  <si>
+    <t>Verify Order History Continue button will load Account page</t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click View your order history under My Orders section -&gt; View Order History -&gt; Click Continue</t>
+  </si>
+  <si>
+    <t>Should be able to view account  page</t>
+  </si>
+  <si>
+    <t>TC_OrderHistory_05</t>
+  </si>
+  <si>
+    <t>Verify UI of order information page</t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click View your order history under My Orders section -&gt; View Order History -&gt; Click  view logo-&gt; View order information-&gt; Check UI</t>
+  </si>
+  <si>
+    <t>TC_OrderHistory_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check add to cart logo of order information page working properly </t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click View your order history under My Orders  section -&gt; View Order History -&gt; Click  view logo-&gt; View order information-&gt; Click add to cart logo</t>
+  </si>
+  <si>
+    <t>Should be able to add products to Add to cart page when add to cart logo will be clicked</t>
+  </si>
+  <si>
+    <t>TC_OrderHistory_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Product Return logo of order information page working properly </t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click View your order history under My Orders section -&gt; View Order History -&gt; Click  view logo-&gt; View order information-&gt; Click product Return logo</t>
+  </si>
+  <si>
+    <t>Should be able to view Product Return page when product return logo will be clicked</t>
+  </si>
+  <si>
+    <t>TC_OrderHistory_08</t>
+  </si>
+  <si>
+    <t>Verify order information Continue button will load Order History page</t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click View your order history under My Orders section -&gt; View Order History -&gt; Click  view logo-&gt; View order information-&gt; Click Continue</t>
+  </si>
+  <si>
+    <t>Should be able to view Order History  page</t>
+  </si>
+  <si>
+    <t>TC_OrderHistory_09</t>
+  </si>
+  <si>
+    <t>Check Order History page is secure</t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click View your order history under My Orders section -&gt; View Order History -&gt; View URL field-&gt; Check lock logo beside URL field</t>
+  </si>
+  <si>
+    <t>TC_OrderHistory_10</t>
+  </si>
+  <si>
+    <t>Check Order Information page is secure</t>
+  </si>
+  <si>
+    <t>View My Account page -&gt; Click View your order history under My Orders section -&gt; View Order History -&gt; Click  view logo-&gt; View order information-&gt;  View URL field-&gt; Check lock logo beside URL field</t>
+  </si>
+  <si>
+    <t>Test Cases For Order History</t>
   </si>
 </sst>
 </file>
@@ -1693,7 +1959,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1824,6 +2090,36 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FD5F1"/>
+        <bgColor rgb="FF9FD5F1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE598"/>
+        <bgColor rgb="FFFFE598"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7CAAC"/>
+        <bgColor rgb="FFF7CAAC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0E0E3"/>
+        <bgColor rgb="FFD0E0E3"/>
       </patternFill>
     </fill>
   </fills>
@@ -1992,7 +2288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2152,6 +2448,12 @@
     <xf numFmtId="0" fontId="8" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2162,11 +2464,26 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3267,14 +3584,14 @@
   </cols>
   <sheetData>
     <row r="7" spans="4:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="57"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="4:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D8" s="33" t="s">
@@ -3620,14 +3937,14 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:8" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="60" t="s">
         <v>280</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
     </row>
     <row r="9" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C9" s="33" t="s">
@@ -4387,7 +4704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C7:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -4402,7 +4719,7 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:8" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="56" t="s">
         <v>337</v>
       </c>
     </row>
@@ -4456,7 +4773,7 @@
       <c r="E11" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="F11" s="61" t="s">
+      <c r="F11" s="55" t="s">
         <v>309</v>
       </c>
       <c r="G11" s="23" t="s">
@@ -4536,7 +4853,7 @@
       <c r="E15" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="F15" s="61" t="s">
+      <c r="F15" s="55" t="s">
         <v>322</v>
       </c>
       <c r="G15" s="23" t="s">
@@ -4576,7 +4893,7 @@
       <c r="E17" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="F17" s="61" t="s">
+      <c r="F17" s="55" t="s">
         <v>329</v>
       </c>
       <c r="G17" s="23" t="s">
@@ -4642,4 +4959,526 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:I17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="44.21875" customWidth="1"/>
+    <col min="7" max="7" width="26.21875" customWidth="1"/>
+    <col min="8" max="8" width="41.6640625" customWidth="1"/>
+    <col min="9" max="9" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="65"/>
+      <c r="F5" s="66" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D7" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="D8" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="E8" s="63" t="s">
+        <v>339</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>341</v>
+      </c>
+      <c r="I8" s="64" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="216" x14ac:dyDescent="0.3">
+      <c r="D9" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>344</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="I9" s="64" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="D10" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>348</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="I10" s="64" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="D11" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>352</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>353</v>
+      </c>
+      <c r="I11" s="64" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="D12" s="34" t="s">
+        <v>355</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>356</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="I12" s="64" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D13" s="34" t="s">
+        <v>359</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>360</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>361</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="D14" s="34" t="s">
+        <v>363</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>364</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>365</v>
+      </c>
+      <c r="I14" s="64" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="D15" s="34" t="s">
+        <v>367</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>368</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>369</v>
+      </c>
+      <c r="I15" s="64" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="D16" s="34" t="s">
+        <v>371</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>372</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="I16" s="64" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="D17" s="34" t="s">
+        <v>375</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>376</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="I17" s="64" t="s">
+        <v>378</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F8" r:id="rId1"/>
+    <hyperlink ref="F9" r:id="rId2"/>
+    <hyperlink ref="F10" r:id="rId3"/>
+    <hyperlink ref="F11" r:id="rId4"/>
+    <hyperlink ref="F12" r:id="rId5"/>
+    <hyperlink ref="F13" r:id="rId6"/>
+    <hyperlink ref="F14" r:id="rId7"/>
+    <hyperlink ref="F15" r:id="rId8"/>
+    <hyperlink ref="F16" r:id="rId9"/>
+    <hyperlink ref="F17" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="5" max="5" width="38.109375" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" customWidth="1"/>
+    <col min="7" max="7" width="52.5546875" customWidth="1"/>
+    <col min="8" max="8" width="37.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="66" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C7" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="C8" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>381</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F8" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="H8" s="69" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="C9" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="D9" s="67" t="s">
+        <v>384</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F9" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="H9" s="69" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="C10" s="23" t="s">
+        <v>387</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>388</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F10" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="H10" s="69" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="C11" s="23" t="s">
+        <v>391</v>
+      </c>
+      <c r="D11" s="67" t="s">
+        <v>392</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F11" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>393</v>
+      </c>
+      <c r="H11" s="69" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="C12" s="23" t="s">
+        <v>395</v>
+      </c>
+      <c r="D12" s="67" t="s">
+        <v>396</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F12" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>397</v>
+      </c>
+      <c r="H12" s="69" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="C13" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="D13" s="67" t="s">
+        <v>399</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F13" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>400</v>
+      </c>
+      <c r="H13" s="69" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="C14" s="23" t="s">
+        <v>402</v>
+      </c>
+      <c r="D14" s="67" t="s">
+        <v>403</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="H14" s="69" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="C15" s="23" t="s">
+        <v>406</v>
+      </c>
+      <c r="D15" s="67" t="s">
+        <v>407</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F15" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>408</v>
+      </c>
+      <c r="H15" s="69" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" ht="288" x14ac:dyDescent="0.3">
+      <c r="C16" s="23" t="s">
+        <v>410</v>
+      </c>
+      <c r="D16" s="67" t="s">
+        <v>411</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F16" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>412</v>
+      </c>
+      <c r="H16" s="69" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="C17" s="23" t="s">
+        <v>413</v>
+      </c>
+      <c r="D17" s="67" t="s">
+        <v>414</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>340</v>
+      </c>
+      <c r="F17" s="68" t="s">
+        <v>283</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>415</v>
+      </c>
+      <c r="H17" s="69" t="s">
+        <v>374</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E8" r:id="rId1"/>
+    <hyperlink ref="E9" r:id="rId2"/>
+    <hyperlink ref="E10" r:id="rId3"/>
+    <hyperlink ref="E11" r:id="rId4"/>
+    <hyperlink ref="E12" r:id="rId5"/>
+    <hyperlink ref="E13" r:id="rId6"/>
+    <hyperlink ref="E14" r:id="rId7"/>
+    <hyperlink ref="E15" r:id="rId8"/>
+    <hyperlink ref="E16" r:id="rId9"/>
+    <hyperlink ref="E17" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>